<commit_message>
add end visit feature
</commit_message>
<xml_diff>
--- a/Resources/DailyLog.xlsx
+++ b/Resources/DailyLog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudio\repos\PackNmove\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65C3635-9A6B-4022-BC27-0ABAF688D218}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19954DBC-C6F0-4F78-91D9-DCA89BF9A962}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1545" yWindow="-120" windowWidth="19065" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>مجموع الزيارات</t>
   </si>
@@ -71,6 +71,9 @@
   <si>
     <t xml:space="preserve">سجل الزيارات الخاص بيوم  </t>
   </si>
+  <si>
+    <t>Visit type</t>
+  </si>
 </sst>
 </file>
 
@@ -79,7 +82,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +141,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -192,7 +202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -257,15 +267,64 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -291,7 +350,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>423333</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>296333</xdr:rowOff>
+      <xdr:rowOff>282725</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -599,10 +658,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J143"/>
+  <dimension ref="A1:K143"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -616,10 +675,11 @@
     <col min="7" max="7" width="29.5703125" style="13" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" style="13" customWidth="1"/>
     <col min="9" max="9" width="19.85546875" style="13" customWidth="1"/>
-    <col min="10" max="10" width="17" style="18" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" style="26" customWidth="1"/>
+    <col min="11" max="11" width="14" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
@@ -628,38 +688,40 @@
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
-      <c r="J1"/>
-    </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="K1"/>
+    </row>
+    <row r="2" spans="1:11" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B2"/>
       <c r="C2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2"/>
-    </row>
-    <row r="3" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="27"/>
+      <c r="K2"/>
+    </row>
+    <row r="3" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3"/>
       <c r="C3" s="12">
-        <f>COUNTA(J5:J152)</f>
+        <f>COUNTA(K5:K152)</f>
         <v>0</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3"/>
-    </row>
-    <row r="4" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="27"/>
+      <c r="K3"/>
+    </row>
+    <row r="4" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>9</v>
       </c>
@@ -687,11 +749,14 @@
       <c r="I4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20"/>
@@ -701,9 +766,10 @@
       <c r="G5" s="20"/>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
-      <c r="J5" s="23"/>
-    </row>
-    <row r="6" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="30"/>
+      <c r="K5" s="32"/>
+    </row>
+    <row r="6" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="19"/>
       <c r="C6" s="20"/>
@@ -713,9 +779,10 @@
       <c r="G6" s="20"/>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
-      <c r="J6" s="23"/>
-    </row>
-    <row r="7" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="30"/>
+      <c r="K6" s="32"/>
+    </row>
+    <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
@@ -725,9 +792,10 @@
       <c r="G7" s="20"/>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
-      <c r="J7" s="23"/>
-    </row>
-    <row r="8" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="30"/>
+      <c r="K7" s="32"/>
+    </row>
+    <row r="8" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19"/>
       <c r="B8" s="19"/>
       <c r="C8" s="20"/>
@@ -737,9 +805,10 @@
       <c r="G8" s="20"/>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
-      <c r="J8" s="23"/>
-    </row>
-    <row r="9" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="30"/>
+      <c r="K8" s="32"/>
+    </row>
+    <row r="9" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="20"/>
@@ -749,9 +818,10 @@
       <c r="G9" s="20"/>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
-      <c r="J9" s="23"/>
-    </row>
-    <row r="10" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="30"/>
+      <c r="K9" s="32"/>
+    </row>
+    <row r="10" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
@@ -761,9 +831,10 @@
       <c r="G10" s="20"/>
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
-      <c r="J10" s="23"/>
-    </row>
-    <row r="11" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="30"/>
+      <c r="K10" s="32"/>
+    </row>
+    <row r="11" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -773,9 +844,10 @@
       <c r="G11" s="20"/>
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
-      <c r="J11" s="23"/>
-    </row>
-    <row r="12" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="30"/>
+      <c r="K11" s="32"/>
+    </row>
+    <row r="12" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="20"/>
@@ -785,9 +857,10 @@
       <c r="G12" s="20"/>
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
-      <c r="J12" s="23"/>
-    </row>
-    <row r="13" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="30"/>
+      <c r="K12" s="32"/>
+    </row>
+    <row r="13" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="20"/>
@@ -797,9 +870,10 @@
       <c r="G13" s="20"/>
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
-      <c r="J13" s="23"/>
-    </row>
-    <row r="14" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="30"/>
+      <c r="K13" s="32"/>
+    </row>
+    <row r="14" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19"/>
       <c r="B14" s="19"/>
       <c r="C14" s="20"/>
@@ -809,9 +883,10 @@
       <c r="G14" s="20"/>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
-      <c r="J14" s="23"/>
-    </row>
-    <row r="15" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="30"/>
+      <c r="K14" s="32"/>
+    </row>
+    <row r="15" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19"/>
       <c r="B15" s="19"/>
       <c r="C15" s="20"/>
@@ -821,9 +896,10 @@
       <c r="G15" s="20"/>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
-      <c r="J15" s="23"/>
-    </row>
-    <row r="16" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="30"/>
+      <c r="K15" s="32"/>
+    </row>
+    <row r="16" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19"/>
       <c r="B16" s="19"/>
       <c r="C16" s="20"/>
@@ -833,9 +909,10 @@
       <c r="G16" s="20"/>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
-      <c r="J16" s="23"/>
-    </row>
-    <row r="17" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="30"/>
+      <c r="K16" s="32"/>
+    </row>
+    <row r="17" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19"/>
       <c r="B17" s="19"/>
       <c r="C17" s="20"/>
@@ -845,9 +922,10 @@
       <c r="G17" s="20"/>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
-      <c r="J17" s="23"/>
-    </row>
-    <row r="18" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="30"/>
+      <c r="K17" s="32"/>
+    </row>
+    <row r="18" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19"/>
       <c r="B18" s="19"/>
       <c r="C18" s="20"/>
@@ -857,9 +935,10 @@
       <c r="G18" s="20"/>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
-      <c r="J18" s="23"/>
-    </row>
-    <row r="19" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J18" s="30"/>
+      <c r="K18" s="32"/>
+    </row>
+    <row r="19" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
       <c r="B19" s="19"/>
       <c r="C19" s="20"/>
@@ -869,9 +948,10 @@
       <c r="G19" s="20"/>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
-      <c r="J19" s="23"/>
-    </row>
-    <row r="20" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J19" s="30"/>
+      <c r="K19" s="32"/>
+    </row>
+    <row r="20" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="20"/>
@@ -881,9 +961,10 @@
       <c r="G20" s="20"/>
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
-      <c r="J20" s="23"/>
-    </row>
-    <row r="21" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="30"/>
+      <c r="K20" s="32"/>
+    </row>
+    <row r="21" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="20"/>
@@ -893,9 +974,10 @@
       <c r="G21" s="20"/>
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
-      <c r="J21" s="23"/>
-    </row>
-    <row r="22" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J21" s="30"/>
+      <c r="K21" s="32"/>
+    </row>
+    <row r="22" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="20"/>
@@ -905,9 +987,10 @@
       <c r="G22" s="20"/>
       <c r="H22" s="19"/>
       <c r="I22" s="19"/>
-      <c r="J22" s="23"/>
-    </row>
-    <row r="23" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J22" s="30"/>
+      <c r="K22" s="32"/>
+    </row>
+    <row r="23" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="19"/>
       <c r="C23" s="20"/>
@@ -917,9 +1000,10 @@
       <c r="G23" s="20"/>
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
-      <c r="J23" s="23"/>
-    </row>
-    <row r="24" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="30"/>
+      <c r="K23" s="32"/>
+    </row>
+    <row r="24" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="19"/>
       <c r="C24" s="20"/>
@@ -929,9 +1013,10 @@
       <c r="G24" s="20"/>
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
-      <c r="J24" s="23"/>
-    </row>
-    <row r="25" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="30"/>
+      <c r="K24" s="32"/>
+    </row>
+    <row r="25" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="19"/>
       <c r="C25" s="20"/>
@@ -941,9 +1026,10 @@
       <c r="G25" s="20"/>
       <c r="H25" s="19"/>
       <c r="I25" s="19"/>
-      <c r="J25" s="23"/>
-    </row>
-    <row r="26" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="30"/>
+      <c r="K25" s="32"/>
+    </row>
+    <row r="26" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="19"/>
       <c r="C26" s="20"/>
@@ -953,9 +1039,10 @@
       <c r="G26" s="20"/>
       <c r="H26" s="19"/>
       <c r="I26" s="19"/>
-      <c r="J26" s="23"/>
-    </row>
-    <row r="27" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="30"/>
+      <c r="K26" s="32"/>
+    </row>
+    <row r="27" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="19"/>
       <c r="C27" s="20"/>
@@ -965,9 +1052,10 @@
       <c r="G27" s="20"/>
       <c r="H27" s="19"/>
       <c r="I27" s="19"/>
-      <c r="J27" s="23"/>
-    </row>
-    <row r="28" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J27" s="30"/>
+      <c r="K27" s="32"/>
+    </row>
+    <row r="28" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="19"/>
       <c r="C28" s="20"/>
@@ -977,9 +1065,10 @@
       <c r="G28" s="20"/>
       <c r="H28" s="19"/>
       <c r="I28" s="19"/>
-      <c r="J28" s="23"/>
-    </row>
-    <row r="29" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J28" s="30"/>
+      <c r="K28" s="32"/>
+    </row>
+    <row r="29" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="19"/>
       <c r="C29" s="20"/>
@@ -989,9 +1078,10 @@
       <c r="G29" s="20"/>
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
-      <c r="J29" s="23"/>
-    </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J29" s="30"/>
+      <c r="K29" s="32"/>
+    </row>
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
       <c r="D30" s="21"/>
@@ -1000,9 +1090,10 @@
       <c r="G30" s="20"/>
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
-      <c r="J30" s="23"/>
-    </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J30" s="20"/>
+      <c r="K30" s="23"/>
+    </row>
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
       <c r="D31" s="21"/>
@@ -1011,9 +1102,10 @@
       <c r="G31" s="20"/>
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
-      <c r="J31" s="23"/>
-    </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J31" s="20"/>
+      <c r="K31" s="23"/>
+    </row>
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
       <c r="D32" s="21"/>
@@ -1022,9 +1114,10 @@
       <c r="G32" s="20"/>
       <c r="H32" s="19"/>
       <c r="I32" s="19"/>
-      <c r="J32" s="23"/>
-    </row>
-    <row r="33" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J32" s="20"/>
+      <c r="K32" s="23"/>
+    </row>
+    <row r="33" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
       <c r="D33" s="21"/>
@@ -1033,9 +1126,10 @@
       <c r="G33" s="20"/>
       <c r="H33" s="19"/>
       <c r="I33" s="19"/>
-      <c r="J33" s="23"/>
-    </row>
-    <row r="34" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J33" s="20"/>
+      <c r="K33" s="23"/>
+    </row>
+    <row r="34" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
       <c r="D34" s="21"/>
@@ -1044,9 +1138,10 @@
       <c r="G34" s="20"/>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
-      <c r="J34" s="23"/>
-    </row>
-    <row r="35" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J34" s="20"/>
+      <c r="K34" s="23"/>
+    </row>
+    <row r="35" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="11"/>
@@ -1055,9 +1150,10 @@
       <c r="G35" s="5"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
-      <c r="J35" s="6"/>
-    </row>
-    <row r="36" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J35" s="5"/>
+      <c r="K35" s="6"/>
+    </row>
+    <row r="36" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="11"/>
@@ -1066,9 +1162,10 @@
       <c r="G36" s="5"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
-      <c r="J36" s="6"/>
-    </row>
-    <row r="37" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J36" s="5"/>
+      <c r="K36" s="6"/>
+    </row>
+    <row r="37" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="11"/>
@@ -1077,9 +1174,10 @@
       <c r="G37" s="5"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
-      <c r="J37" s="6"/>
-    </row>
-    <row r="38" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J37" s="5"/>
+      <c r="K37" s="6"/>
+    </row>
+    <row r="38" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="11"/>
@@ -1088,9 +1186,10 @@
       <c r="G38" s="5"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
-      <c r="J38" s="6"/>
-    </row>
-    <row r="39" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J38" s="5"/>
+      <c r="K38" s="6"/>
+    </row>
+    <row r="39" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="11"/>
@@ -1099,9 +1198,10 @@
       <c r="G39" s="5"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
-      <c r="J39" s="6"/>
-    </row>
-    <row r="40" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J39" s="5"/>
+      <c r="K39" s="6"/>
+    </row>
+    <row r="40" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="11"/>
@@ -1110,9 +1210,10 @@
       <c r="G40" s="5"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
-      <c r="J40" s="6"/>
-    </row>
-    <row r="41" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J40" s="5"/>
+      <c r="K40" s="6"/>
+    </row>
+    <row r="41" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="11"/>
@@ -1121,9 +1222,10 @@
       <c r="G41" s="5"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
-      <c r="J41" s="6"/>
-    </row>
-    <row r="42" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J41" s="5"/>
+      <c r="K41" s="6"/>
+    </row>
+    <row r="42" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="11"/>
@@ -1132,9 +1234,10 @@
       <c r="G42" s="5"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
-      <c r="J42" s="6"/>
-    </row>
-    <row r="43" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J42" s="5"/>
+      <c r="K42" s="6"/>
+    </row>
+    <row r="43" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="11"/>
@@ -1143,9 +1246,10 @@
       <c r="G43" s="5"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="6"/>
-    </row>
-    <row r="44" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J43" s="5"/>
+      <c r="K43" s="6"/>
+    </row>
+    <row r="44" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="11"/>
@@ -1154,9 +1258,10 @@
       <c r="G44" s="5"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
-      <c r="J44" s="6"/>
-    </row>
-    <row r="45" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J44" s="5"/>
+      <c r="K44" s="6"/>
+    </row>
+    <row r="45" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="11"/>
@@ -1165,9 +1270,10 @@
       <c r="G45" s="5"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
-      <c r="J45" s="6"/>
-    </row>
-    <row r="46" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J45" s="5"/>
+      <c r="K45" s="6"/>
+    </row>
+    <row r="46" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="2"/>
       <c r="D46" s="11"/>
@@ -1176,9 +1282,10 @@
       <c r="G46" s="5"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
-      <c r="J46" s="3"/>
-    </row>
-    <row r="47" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J46" s="29"/>
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="2"/>
       <c r="D47" s="11"/>
@@ -1187,9 +1294,10 @@
       <c r="G47" s="5"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
-      <c r="J47" s="3"/>
-    </row>
-    <row r="48" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J47" s="29"/>
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="2"/>
       <c r="D48" s="11"/>
@@ -1198,9 +1306,10 @@
       <c r="G48" s="5"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
-      <c r="J48" s="3"/>
-    </row>
-    <row r="49" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J48" s="29"/>
+      <c r="K48" s="3"/>
+    </row>
+    <row r="49" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="2"/>
       <c r="D49" s="11"/>
@@ -1209,9 +1318,10 @@
       <c r="G49" s="5"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
-      <c r="J49" s="3"/>
-    </row>
-    <row r="50" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J49" s="29"/>
+      <c r="K49" s="3"/>
+    </row>
+    <row r="50" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="2"/>
       <c r="D50" s="11"/>
@@ -1220,9 +1330,10 @@
       <c r="G50" s="5"/>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
-      <c r="J50" s="3"/>
-    </row>
-    <row r="51" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J50" s="29"/>
+      <c r="K50" s="3"/>
+    </row>
+    <row r="51" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="2"/>
       <c r="D51" s="11"/>
@@ -1231,9 +1342,10 @@
       <c r="G51" s="5"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
-      <c r="J51" s="3"/>
-    </row>
-    <row r="52" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J51" s="29"/>
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="2"/>
       <c r="D52" s="11"/>
@@ -1242,9 +1354,10 @@
       <c r="G52" s="5"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
-      <c r="J52" s="3"/>
-    </row>
-    <row r="53" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J52" s="29"/>
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="2"/>
       <c r="D53" s="11"/>
@@ -1253,9 +1366,10 @@
       <c r="G53" s="5"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
-      <c r="J53" s="3"/>
-    </row>
-    <row r="54" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J53" s="29"/>
+      <c r="K53" s="3"/>
+    </row>
+    <row r="54" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="2"/>
       <c r="D54" s="11"/>
@@ -1264,9 +1378,10 @@
       <c r="G54" s="5"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
-      <c r="J54" s="3"/>
-    </row>
-    <row r="55" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J54" s="29"/>
+      <c r="K54" s="3"/>
+    </row>
+    <row r="55" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="2"/>
       <c r="D55" s="11"/>
@@ -1275,9 +1390,10 @@
       <c r="G55" s="5"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
-      <c r="J55" s="3"/>
-    </row>
-    <row r="56" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J55" s="29"/>
+      <c r="K55" s="3"/>
+    </row>
+    <row r="56" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="2"/>
       <c r="D56" s="11"/>
@@ -1286,9 +1402,10 @@
       <c r="G56" s="5"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
-      <c r="J56" s="3"/>
-    </row>
-    <row r="57" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J56" s="29"/>
+      <c r="K56" s="3"/>
+    </row>
+    <row r="57" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="C57" s="2"/>
       <c r="D57" s="11"/>
@@ -1297,9 +1414,10 @@
       <c r="G57" s="5"/>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
-      <c r="J57" s="3"/>
-    </row>
-    <row r="58" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J57" s="29"/>
+      <c r="K57" s="3"/>
+    </row>
+    <row r="58" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58" s="2"/>
       <c r="D58" s="11"/>
@@ -1308,9 +1426,10 @@
       <c r="G58" s="5"/>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
-      <c r="J58" s="3"/>
-    </row>
-    <row r="59" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J58" s="29"/>
+      <c r="K58" s="3"/>
+    </row>
+    <row r="59" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="C59" s="2"/>
       <c r="D59" s="11"/>
@@ -1319,9 +1438,10 @@
       <c r="G59" s="5"/>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
-      <c r="J59" s="3"/>
-    </row>
-    <row r="60" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J59" s="29"/>
+      <c r="K59" s="3"/>
+    </row>
+    <row r="60" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="C60" s="2"/>
       <c r="D60" s="11"/>
@@ -1330,9 +1450,10 @@
       <c r="G60" s="5"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
-      <c r="J60" s="3"/>
-    </row>
-    <row r="61" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J60" s="29"/>
+      <c r="K60" s="3"/>
+    </row>
+    <row r="61" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="C61" s="2"/>
       <c r="D61" s="11"/>
@@ -1341,9 +1462,10 @@
       <c r="G61" s="5"/>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
-      <c r="J61" s="3"/>
-    </row>
-    <row r="62" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J61" s="29"/>
+      <c r="K61" s="3"/>
+    </row>
+    <row r="62" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="2"/>
       <c r="D62" s="11"/>
@@ -1352,9 +1474,10 @@
       <c r="G62" s="5"/>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
-      <c r="J62" s="3"/>
-    </row>
-    <row r="63" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J62" s="29"/>
+      <c r="K62" s="3"/>
+    </row>
+    <row r="63" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="C63" s="2"/>
       <c r="D63" s="11"/>
@@ -1363,9 +1486,10 @@
       <c r="G63" s="5"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
-      <c r="J63" s="3"/>
-    </row>
-    <row r="64" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J63" s="29"/>
+      <c r="K63" s="3"/>
+    </row>
+    <row r="64" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="C64" s="2"/>
       <c r="D64" s="11"/>
@@ -1374,9 +1498,10 @@
       <c r="G64" s="5"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
-      <c r="J64" s="3"/>
-    </row>
-    <row r="65" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J64" s="29"/>
+      <c r="K64" s="3"/>
+    </row>
+    <row r="65" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="C65" s="2"/>
       <c r="D65" s="11"/>
@@ -1385,9 +1510,10 @@
       <c r="G65" s="5"/>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
-      <c r="J65" s="3"/>
-    </row>
-    <row r="66" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J65" s="29"/>
+      <c r="K65" s="3"/>
+    </row>
+    <row r="66" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="C66" s="2"/>
       <c r="D66" s="11"/>
@@ -1396,9 +1522,10 @@
       <c r="G66" s="5"/>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
-      <c r="J66" s="3"/>
-    </row>
-    <row r="67" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J66" s="29"/>
+      <c r="K66" s="3"/>
+    </row>
+    <row r="67" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
       <c r="C67" s="2"/>
       <c r="D67" s="11"/>
@@ -1407,9 +1534,10 @@
       <c r="G67" s="5"/>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
-      <c r="J67" s="3"/>
-    </row>
-    <row r="68" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J67" s="29"/>
+      <c r="K67" s="3"/>
+    </row>
+    <row r="68" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
       <c r="C68" s="2"/>
       <c r="D68" s="11"/>
@@ -1418,9 +1546,10 @@
       <c r="G68" s="5"/>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
-      <c r="J68" s="3"/>
-    </row>
-    <row r="69" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J68" s="29"/>
+      <c r="K68" s="3"/>
+    </row>
+    <row r="69" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="C69" s="2"/>
       <c r="D69" s="11"/>
@@ -1429,9 +1558,10 @@
       <c r="G69" s="5"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
-      <c r="J69" s="3"/>
-    </row>
-    <row r="70" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J69" s="29"/>
+      <c r="K69" s="3"/>
+    </row>
+    <row r="70" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="C70" s="2"/>
       <c r="D70" s="11"/>
@@ -1440,9 +1570,10 @@
       <c r="G70" s="5"/>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
-      <c r="J70" s="3"/>
-    </row>
-    <row r="71" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J70" s="29"/>
+      <c r="K70" s="3"/>
+    </row>
+    <row r="71" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="C71" s="2"/>
       <c r="D71" s="11"/>
@@ -1451,9 +1582,10 @@
       <c r="G71" s="5"/>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
-      <c r="J71" s="3"/>
-    </row>
-    <row r="72" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J71" s="29"/>
+      <c r="K71" s="3"/>
+    </row>
+    <row r="72" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="C72" s="2"/>
       <c r="D72" s="11"/>
@@ -1462,9 +1594,10 @@
       <c r="G72" s="5"/>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
-      <c r="J72" s="3"/>
-    </row>
-    <row r="73" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J72" s="29"/>
+      <c r="K72" s="3"/>
+    </row>
+    <row r="73" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="C73" s="2"/>
       <c r="D73" s="11"/>
@@ -1473,9 +1606,10 @@
       <c r="G73" s="5"/>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
-      <c r="J73" s="3"/>
-    </row>
-    <row r="74" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J73" s="29"/>
+      <c r="K73" s="3"/>
+    </row>
+    <row r="74" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
       <c r="C74" s="2"/>
       <c r="D74" s="11"/>
@@ -1484,9 +1618,10 @@
       <c r="G74" s="5"/>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
-      <c r="J74" s="3"/>
-    </row>
-    <row r="75" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J74" s="29"/>
+      <c r="K74" s="3"/>
+    </row>
+    <row r="75" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B75" s="1"/>
       <c r="C75" s="2"/>
       <c r="D75" s="11"/>
@@ -1495,9 +1630,10 @@
       <c r="G75" s="5"/>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
-      <c r="J75" s="3"/>
-    </row>
-    <row r="76" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J75" s="29"/>
+      <c r="K75" s="3"/>
+    </row>
+    <row r="76" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="C76" s="2"/>
       <c r="D76" s="11"/>
@@ -1506,9 +1642,10 @@
       <c r="G76" s="5"/>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
-      <c r="J76" s="3"/>
-    </row>
-    <row r="77" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J76" s="29"/>
+      <c r="K76" s="3"/>
+    </row>
+    <row r="77" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="C77" s="2"/>
       <c r="D77" s="11"/>
@@ -1517,9 +1654,10 @@
       <c r="G77" s="5"/>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
-      <c r="J77" s="3"/>
-    </row>
-    <row r="78" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J77" s="29"/>
+      <c r="K77" s="3"/>
+    </row>
+    <row r="78" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="C78" s="2"/>
       <c r="D78" s="11"/>
@@ -1528,9 +1666,10 @@
       <c r="G78" s="5"/>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
-      <c r="J78" s="3"/>
-    </row>
-    <row r="79" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J78" s="29"/>
+      <c r="K78" s="3"/>
+    </row>
+    <row r="79" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
       <c r="C79" s="2"/>
       <c r="D79" s="11"/>
@@ -1539,9 +1678,10 @@
       <c r="G79" s="5"/>
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
-      <c r="J79" s="3"/>
-    </row>
-    <row r="80" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J79" s="29"/>
+      <c r="K79" s="3"/>
+    </row>
+    <row r="80" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="C80" s="2"/>
       <c r="D80" s="11"/>
@@ -1550,9 +1690,10 @@
       <c r="G80" s="5"/>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
-      <c r="J80" s="3"/>
-    </row>
-    <row r="81" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J80" s="29"/>
+      <c r="K80" s="3"/>
+    </row>
+    <row r="81" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
       <c r="C81" s="2"/>
       <c r="D81" s="11"/>
@@ -1561,9 +1702,10 @@
       <c r="G81" s="5"/>
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
-      <c r="J81" s="3"/>
-    </row>
-    <row r="82" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J81" s="29"/>
+      <c r="K81" s="3"/>
+    </row>
+    <row r="82" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="C82" s="2"/>
       <c r="D82" s="11"/>
@@ -1572,9 +1714,10 @@
       <c r="G82" s="5"/>
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
-      <c r="J82" s="3"/>
-    </row>
-    <row r="83" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J82" s="29"/>
+      <c r="K82" s="3"/>
+    </row>
+    <row r="83" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="C83" s="2"/>
       <c r="D83" s="11"/>
@@ -1583,9 +1726,10 @@
       <c r="G83" s="5"/>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
-      <c r="J83" s="3"/>
-    </row>
-    <row r="84" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J83" s="29"/>
+      <c r="K83" s="3"/>
+    </row>
+    <row r="84" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
       <c r="C84" s="2"/>
       <c r="D84" s="11"/>
@@ -1594,9 +1738,10 @@
       <c r="G84" s="5"/>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
-      <c r="J84" s="3"/>
-    </row>
-    <row r="85" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J84" s="29"/>
+      <c r="K84" s="3"/>
+    </row>
+    <row r="85" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="C85" s="2"/>
       <c r="D85" s="11"/>
@@ -1605,9 +1750,10 @@
       <c r="G85" s="5"/>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
-      <c r="J85" s="3"/>
-    </row>
-    <row r="86" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J85" s="29"/>
+      <c r="K85" s="3"/>
+    </row>
+    <row r="86" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B86" s="1"/>
       <c r="C86" s="2"/>
       <c r="D86" s="11"/>
@@ -1616,9 +1762,10 @@
       <c r="G86" s="5"/>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
-      <c r="J86" s="3"/>
-    </row>
-    <row r="87" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J86" s="29"/>
+      <c r="K86" s="3"/>
+    </row>
+    <row r="87" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
       <c r="C87" s="2"/>
       <c r="D87" s="11"/>
@@ -1627,9 +1774,10 @@
       <c r="G87" s="5"/>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
-      <c r="J87" s="3"/>
-    </row>
-    <row r="88" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J87" s="29"/>
+      <c r="K87" s="3"/>
+    </row>
+    <row r="88" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
       <c r="C88" s="2"/>
       <c r="D88" s="11"/>
@@ -1638,9 +1786,10 @@
       <c r="G88" s="5"/>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
-      <c r="J88" s="3"/>
-    </row>
-    <row r="89" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J88" s="29"/>
+      <c r="K88" s="3"/>
+    </row>
+    <row r="89" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
       <c r="C89" s="2"/>
       <c r="D89" s="11"/>
@@ -1649,9 +1798,10 @@
       <c r="G89" s="5"/>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
-      <c r="J89" s="3"/>
-    </row>
-    <row r="90" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J89" s="29"/>
+      <c r="K89" s="3"/>
+    </row>
+    <row r="90" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B90" s="1"/>
       <c r="C90" s="2"/>
       <c r="D90" s="11"/>
@@ -1660,9 +1810,10 @@
       <c r="G90" s="5"/>
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
-      <c r="J90" s="3"/>
-    </row>
-    <row r="91" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J90" s="29"/>
+      <c r="K90" s="3"/>
+    </row>
+    <row r="91" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
       <c r="C91" s="2"/>
       <c r="D91" s="11"/>
@@ -1671,9 +1822,10 @@
       <c r="G91" s="5"/>
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
-      <c r="J91" s="3"/>
-    </row>
-    <row r="92" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J91" s="29"/>
+      <c r="K91" s="3"/>
+    </row>
+    <row r="92" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B92" s="1"/>
       <c r="C92" s="2"/>
       <c r="D92" s="11"/>
@@ -1682,9 +1834,10 @@
       <c r="G92" s="5"/>
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
-      <c r="J92" s="3"/>
-    </row>
-    <row r="93" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J92" s="29"/>
+      <c r="K92" s="3"/>
+    </row>
+    <row r="93" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B93" s="1"/>
       <c r="C93" s="2"/>
       <c r="D93" s="11"/>
@@ -1693,9 +1846,10 @@
       <c r="G93" s="5"/>
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
-      <c r="J93" s="3"/>
-    </row>
-    <row r="94" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J93" s="29"/>
+      <c r="K93" s="3"/>
+    </row>
+    <row r="94" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
       <c r="C94" s="2"/>
       <c r="D94" s="11"/>
@@ -1704,9 +1858,10 @@
       <c r="G94" s="5"/>
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
-      <c r="J94" s="3"/>
-    </row>
-    <row r="95" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J94" s="29"/>
+      <c r="K94" s="3"/>
+    </row>
+    <row r="95" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B95" s="1"/>
       <c r="C95" s="2"/>
       <c r="D95" s="11"/>
@@ -1715,9 +1870,10 @@
       <c r="G95" s="5"/>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
-      <c r="J95" s="3"/>
-    </row>
-    <row r="96" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J95" s="29"/>
+      <c r="K95" s="3"/>
+    </row>
+    <row r="96" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
       <c r="C96" s="2"/>
       <c r="D96" s="11"/>
@@ -1726,9 +1882,10 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
-      <c r="J96" s="3"/>
-    </row>
-    <row r="97" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J96" s="29"/>
+      <c r="K96" s="3"/>
+    </row>
+    <row r="97" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
       <c r="C97" s="2"/>
       <c r="D97" s="11"/>
@@ -1737,9 +1894,10 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
-      <c r="J97" s="3"/>
-    </row>
-    <row r="98" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J97" s="29"/>
+      <c r="K97" s="3"/>
+    </row>
+    <row r="98" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="C98" s="2"/>
       <c r="D98" s="11"/>
@@ -1748,9 +1906,10 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
-      <c r="J98" s="3"/>
-    </row>
-    <row r="99" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J98" s="29"/>
+      <c r="K98" s="3"/>
+    </row>
+    <row r="99" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
       <c r="C99" s="2"/>
       <c r="D99" s="11"/>
@@ -1759,9 +1918,10 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
-      <c r="J99" s="3"/>
-    </row>
-    <row r="100" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J99" s="29"/>
+      <c r="K99" s="3"/>
+    </row>
+    <row r="100" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B100" s="1"/>
       <c r="C100" s="2"/>
       <c r="D100" s="11"/>
@@ -1770,9 +1930,10 @@
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
-      <c r="J100" s="3"/>
-    </row>
-    <row r="101" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J100" s="29"/>
+      <c r="K100" s="3"/>
+    </row>
+    <row r="101" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B101" s="1"/>
       <c r="C101" s="2"/>
       <c r="D101" s="11"/>
@@ -1781,9 +1942,10 @@
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
-      <c r="J101" s="3"/>
-    </row>
-    <row r="102" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J101" s="29"/>
+      <c r="K101" s="3"/>
+    </row>
+    <row r="102" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B102" s="1"/>
       <c r="C102" s="2"/>
       <c r="D102" s="11"/>
@@ -1792,9 +1954,10 @@
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
-      <c r="J102" s="3"/>
-    </row>
-    <row r="103" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J102" s="29"/>
+      <c r="K102" s="3"/>
+    </row>
+    <row r="103" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B103" s="1"/>
       <c r="C103" s="2"/>
       <c r="D103" s="11"/>
@@ -1803,9 +1966,10 @@
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
-      <c r="J103" s="3"/>
-    </row>
-    <row r="104" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J103" s="29"/>
+      <c r="K103" s="3"/>
+    </row>
+    <row r="104" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B104" s="1"/>
       <c r="C104" s="2"/>
       <c r="D104" s="11"/>
@@ -1814,9 +1978,10 @@
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
-      <c r="J104" s="3"/>
-    </row>
-    <row r="105" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J104" s="29"/>
+      <c r="K104" s="3"/>
+    </row>
+    <row r="105" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
       <c r="C105" s="2"/>
       <c r="D105" s="11"/>
@@ -1825,9 +1990,10 @@
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
-      <c r="J105" s="3"/>
-    </row>
-    <row r="106" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J105" s="29"/>
+      <c r="K105" s="3"/>
+    </row>
+    <row r="106" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="C106" s="2"/>
       <c r="D106" s="11"/>
@@ -1836,9 +2002,10 @@
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
-      <c r="J106" s="3"/>
-    </row>
-    <row r="107" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J106" s="29"/>
+      <c r="K106" s="3"/>
+    </row>
+    <row r="107" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="C107" s="2"/>
       <c r="D107" s="11"/>
@@ -1847,9 +2014,10 @@
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
-      <c r="J107" s="3"/>
-    </row>
-    <row r="108" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J107" s="29"/>
+      <c r="K107" s="3"/>
+    </row>
+    <row r="108" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
       <c r="C108" s="2"/>
       <c r="D108" s="11"/>
@@ -1858,9 +2026,10 @@
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
-      <c r="J108" s="3"/>
-    </row>
-    <row r="109" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J108" s="29"/>
+      <c r="K108" s="3"/>
+    </row>
+    <row r="109" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B109" s="1"/>
       <c r="C109" s="2"/>
       <c r="D109" s="11"/>
@@ -1869,9 +2038,10 @@
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
-      <c r="J109" s="3"/>
-    </row>
-    <row r="110" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J109" s="29"/>
+      <c r="K109" s="3"/>
+    </row>
+    <row r="110" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B110" s="1"/>
       <c r="C110" s="2"/>
       <c r="D110" s="11"/>
@@ -1880,9 +2050,10 @@
       <c r="G110" s="2"/>
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
-      <c r="J110" s="3"/>
-    </row>
-    <row r="111" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J110" s="29"/>
+      <c r="K110" s="3"/>
+    </row>
+    <row r="111" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B111" s="1"/>
       <c r="C111" s="2"/>
       <c r="D111" s="11"/>
@@ -1891,9 +2062,10 @@
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
-      <c r="J111" s="3"/>
-    </row>
-    <row r="112" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J111" s="29"/>
+      <c r="K111" s="3"/>
+    </row>
+    <row r="112" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B112" s="1"/>
       <c r="C112" s="2"/>
       <c r="D112" s="11"/>
@@ -1902,9 +2074,10 @@
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
-      <c r="J112" s="3"/>
-    </row>
-    <row r="113" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J112" s="29"/>
+      <c r="K112" s="3"/>
+    </row>
+    <row r="113" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B113" s="1"/>
       <c r="C113" s="2"/>
       <c r="D113" s="11"/>
@@ -1913,9 +2086,10 @@
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
-      <c r="J113" s="3"/>
-    </row>
-    <row r="114" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J113" s="29"/>
+      <c r="K113" s="3"/>
+    </row>
+    <row r="114" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B114" s="1"/>
       <c r="C114" s="2"/>
       <c r="D114" s="11"/>
@@ -1924,9 +2098,10 @@
       <c r="G114" s="2"/>
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
-      <c r="J114" s="3"/>
-    </row>
-    <row r="115" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J114" s="29"/>
+      <c r="K114" s="3"/>
+    </row>
+    <row r="115" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B115" s="1"/>
       <c r="C115" s="2"/>
       <c r="D115" s="7"/>
@@ -1935,9 +2110,10 @@
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
-      <c r="J115" s="3"/>
-    </row>
-    <row r="116" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J115" s="29"/>
+      <c r="K115" s="3"/>
+    </row>
+    <row r="116" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B116" s="1"/>
       <c r="C116" s="2"/>
       <c r="D116" s="7"/>
@@ -1946,9 +2122,10 @@
       <c r="G116" s="2"/>
       <c r="H116" s="2"/>
       <c r="I116" s="2"/>
-      <c r="J116" s="3"/>
-    </row>
-    <row r="117" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J116" s="29"/>
+      <c r="K116" s="3"/>
+    </row>
+    <row r="117" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B117" s="1"/>
       <c r="C117" s="2"/>
       <c r="D117" s="7"/>
@@ -1957,9 +2134,10 @@
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
-      <c r="J117" s="3"/>
-    </row>
-    <row r="118" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J117" s="29"/>
+      <c r="K117" s="3"/>
+    </row>
+    <row r="118" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B118" s="1"/>
       <c r="C118" s="2"/>
       <c r="D118" s="7"/>
@@ -1968,9 +2146,10 @@
       <c r="G118" s="2"/>
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
-      <c r="J118" s="3"/>
-    </row>
-    <row r="119" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J118" s="29"/>
+      <c r="K118" s="3"/>
+    </row>
+    <row r="119" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B119" s="1"/>
       <c r="C119" s="2"/>
       <c r="D119" s="7"/>
@@ -1979,9 +2158,10 @@
       <c r="G119" s="2"/>
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
-      <c r="J119" s="3"/>
-    </row>
-    <row r="120" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J119" s="29"/>
+      <c r="K119" s="3"/>
+    </row>
+    <row r="120" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B120" s="1"/>
       <c r="C120" s="2"/>
       <c r="D120" s="7"/>
@@ -1990,9 +2170,10 @@
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
-      <c r="J120" s="3"/>
-    </row>
-    <row r="121" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J120" s="29"/>
+      <c r="K120" s="3"/>
+    </row>
+    <row r="121" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B121" s="1"/>
       <c r="C121" s="2"/>
       <c r="D121" s="7"/>
@@ -2001,9 +2182,10 @@
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
-      <c r="J121" s="3"/>
-    </row>
-    <row r="122" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J121" s="29"/>
+      <c r="K121" s="3"/>
+    </row>
+    <row r="122" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B122" s="1"/>
       <c r="C122" s="2"/>
       <c r="D122" s="7"/>
@@ -2012,9 +2194,10 @@
       <c r="G122" s="2"/>
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
-      <c r="J122" s="3"/>
-    </row>
-    <row r="123" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J122" s="29"/>
+      <c r="K122" s="3"/>
+    </row>
+    <row r="123" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B123" s="1"/>
       <c r="C123" s="2"/>
       <c r="D123" s="7"/>
@@ -2023,9 +2206,10 @@
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
-      <c r="J123" s="3"/>
-    </row>
-    <row r="124" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J123" s="29"/>
+      <c r="K123" s="3"/>
+    </row>
+    <row r="124" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B124" s="1"/>
       <c r="C124" s="2"/>
       <c r="D124" s="7"/>
@@ -2034,9 +2218,10 @@
       <c r="G124" s="2"/>
       <c r="H124" s="2"/>
       <c r="I124" s="2"/>
-      <c r="J124" s="3"/>
-    </row>
-    <row r="125" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J124" s="29"/>
+      <c r="K124" s="3"/>
+    </row>
+    <row r="125" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B125" s="1"/>
       <c r="C125" s="2"/>
       <c r="D125" s="7"/>
@@ -2045,9 +2230,10 @@
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
-      <c r="J125" s="3"/>
-    </row>
-    <row r="126" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J125" s="29"/>
+      <c r="K125" s="3"/>
+    </row>
+    <row r="126" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B126" s="1"/>
       <c r="C126" s="2"/>
       <c r="D126" s="7"/>
@@ -2056,9 +2242,10 @@
       <c r="G126" s="2"/>
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
-      <c r="J126" s="3"/>
-    </row>
-    <row r="127" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J126" s="29"/>
+      <c r="K126" s="3"/>
+    </row>
+    <row r="127" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B127" s="1"/>
       <c r="C127" s="2"/>
       <c r="D127" s="7"/>
@@ -2067,9 +2254,10 @@
       <c r="G127" s="2"/>
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
-      <c r="J127" s="3"/>
-    </row>
-    <row r="128" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J127" s="29"/>
+      <c r="K127" s="3"/>
+    </row>
+    <row r="128" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B128" s="1"/>
       <c r="C128" s="2"/>
       <c r="D128" s="7"/>
@@ -2078,9 +2266,10 @@
       <c r="G128" s="2"/>
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
-      <c r="J128" s="3"/>
-    </row>
-    <row r="129" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J128" s="29"/>
+      <c r="K128" s="3"/>
+    </row>
+    <row r="129" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B129" s="1"/>
       <c r="C129" s="2"/>
       <c r="D129" s="7"/>
@@ -2089,9 +2278,10 @@
       <c r="G129" s="2"/>
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
-      <c r="J129" s="3"/>
-    </row>
-    <row r="130" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J129" s="29"/>
+      <c r="K129" s="3"/>
+    </row>
+    <row r="130" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B130" s="1"/>
       <c r="C130" s="2"/>
       <c r="D130" s="7"/>
@@ -2100,9 +2290,10 @@
       <c r="G130" s="2"/>
       <c r="H130" s="2"/>
       <c r="I130" s="2"/>
-      <c r="J130" s="3"/>
-    </row>
-    <row r="131" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J130" s="29"/>
+      <c r="K130" s="3"/>
+    </row>
+    <row r="131" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B131" s="1"/>
       <c r="C131" s="2"/>
       <c r="D131" s="7"/>
@@ -2111,9 +2302,10 @@
       <c r="G131" s="2"/>
       <c r="H131" s="2"/>
       <c r="I131" s="2"/>
-      <c r="J131" s="3"/>
-    </row>
-    <row r="132" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J131" s="29"/>
+      <c r="K131" s="3"/>
+    </row>
+    <row r="132" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B132" s="1"/>
       <c r="C132" s="2"/>
       <c r="D132" s="7"/>
@@ -2122,9 +2314,10 @@
       <c r="G132" s="2"/>
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
-      <c r="J132" s="3"/>
-    </row>
-    <row r="133" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J132" s="29"/>
+      <c r="K132" s="3"/>
+    </row>
+    <row r="133" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B133" s="1"/>
       <c r="C133" s="2"/>
       <c r="D133" s="7"/>
@@ -2133,9 +2326,10 @@
       <c r="G133" s="2"/>
       <c r="H133" s="2"/>
       <c r="I133" s="2"/>
-      <c r="J133" s="3"/>
-    </row>
-    <row r="134" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J133" s="29"/>
+      <c r="K133" s="3"/>
+    </row>
+    <row r="134" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B134" s="1"/>
       <c r="C134" s="2"/>
       <c r="D134" s="7"/>
@@ -2144,9 +2338,10 @@
       <c r="G134" s="2"/>
       <c r="H134" s="2"/>
       <c r="I134" s="2"/>
-      <c r="J134" s="3"/>
-    </row>
-    <row r="135" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J134" s="29"/>
+      <c r="K134" s="3"/>
+    </row>
+    <row r="135" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B135" s="1"/>
       <c r="C135" s="2"/>
       <c r="D135" s="7"/>
@@ -2155,9 +2350,10 @@
       <c r="G135" s="2"/>
       <c r="H135" s="2"/>
       <c r="I135" s="2"/>
-      <c r="J135" s="3"/>
-    </row>
-    <row r="136" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J135" s="29"/>
+      <c r="K135" s="3"/>
+    </row>
+    <row r="136" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B136" s="1"/>
       <c r="C136" s="2"/>
       <c r="D136" s="7"/>
@@ -2166,9 +2362,10 @@
       <c r="G136" s="2"/>
       <c r="H136" s="2"/>
       <c r="I136" s="2"/>
-      <c r="J136" s="3"/>
-    </row>
-    <row r="137" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J136" s="29"/>
+      <c r="K136" s="3"/>
+    </row>
+    <row r="137" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B137" s="1"/>
       <c r="C137" s="2"/>
       <c r="D137" s="7"/>
@@ -2177,9 +2374,10 @@
       <c r="G137" s="2"/>
       <c r="H137" s="2"/>
       <c r="I137" s="2"/>
-      <c r="J137" s="3"/>
-    </row>
-    <row r="138" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J137" s="29"/>
+      <c r="K137" s="3"/>
+    </row>
+    <row r="138" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="C138" s="14"/>
       <c r="D138" s="15"/>
       <c r="E138" s="9"/>
@@ -2187,9 +2385,10 @@
       <c r="G138" s="14"/>
       <c r="H138" s="14"/>
       <c r="I138" s="14"/>
-      <c r="J138" s="16"/>
-    </row>
-    <row r="139" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J138" s="29"/>
+      <c r="K138" s="16"/>
+    </row>
+    <row r="139" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="C139" s="14"/>
       <c r="D139" s="15"/>
       <c r="E139" s="9"/>
@@ -2197,9 +2396,10 @@
       <c r="G139" s="14"/>
       <c r="H139" s="14"/>
       <c r="I139" s="14"/>
-      <c r="J139" s="16"/>
-    </row>
-    <row r="140" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J139" s="29"/>
+      <c r="K139" s="16"/>
+    </row>
+    <row r="140" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="C140" s="14"/>
       <c r="D140" s="15"/>
       <c r="E140" s="9"/>
@@ -2207,9 +2407,10 @@
       <c r="G140" s="14"/>
       <c r="H140" s="14"/>
       <c r="I140" s="14"/>
-      <c r="J140" s="16"/>
-    </row>
-    <row r="141" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J140" s="29"/>
+      <c r="K140" s="16"/>
+    </row>
+    <row r="141" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="C141" s="14"/>
       <c r="D141" s="15"/>
       <c r="E141" s="9"/>
@@ -2217,9 +2418,10 @@
       <c r="G141" s="14"/>
       <c r="H141" s="14"/>
       <c r="I141" s="14"/>
-      <c r="J141" s="16"/>
-    </row>
-    <row r="142" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J141" s="29"/>
+      <c r="K141" s="16"/>
+    </row>
+    <row r="142" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="C142" s="14"/>
       <c r="D142" s="15"/>
       <c r="E142" s="9"/>
@@ -2227,9 +2429,10 @@
       <c r="G142" s="14"/>
       <c r="H142" s="14"/>
       <c r="I142" s="14"/>
-      <c r="J142" s="16"/>
-    </row>
-    <row r="143" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J142" s="29"/>
+      <c r="K142" s="16"/>
+    </row>
+    <row r="143" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="C143" s="14"/>
       <c r="D143" s="15"/>
       <c r="E143" s="9"/>
@@ -2237,14 +2440,23 @@
       <c r="G143" s="14"/>
       <c r="H143" s="14"/>
       <c r="I143" s="14"/>
-      <c r="J143" s="16"/>
+      <c r="J143" s="29"/>
+      <c r="K143" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D2:I3"/>
   </mergeCells>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="دخو">
+      <formula>NOT(ISERROR(SEARCH("دخو",K1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="خرو">
+      <formula>NOT(ISERROR(SEARCH("خرو",K1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="76" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="72" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>